<commit_message>
Scheduled quarters, added proposed dispositions.
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@2179 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/ballots/2013-09 DSTU/QA/FHIR DSTU Review Template - Lloyd.xlsx
+++ b/ballots/2013-09 DSTU/QA/FHIR DSTU Review Template - Lloyd.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="825" windowWidth="25740" windowHeight="14910" activeTab="2"/>
+    <workbookView xWindow="3405" yWindow="825" windowWidth="25740" windowHeight="14910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Reconciliation Peer Review" sheetId="2" r:id="rId2"/>
     <sheet name="Specification QA" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
   <si>
     <t>Reviewer Name</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>done the note. Implementation collateral to follow after San Antonio</t>
+  </si>
+  <si>
+    <t>The ballot comment was misunderstood.  Conformance still needs to declare what search parameters will be supported.  However, Profile should be used to *define* search parameters - you want the search parameters to be able to be defined the same place you define the resource element or extension being searched on.</t>
   </si>
 </sst>
 </file>
@@ -782,13 +785,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +801,7 @@
     <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -807,6 +810,20 @@
       </c>
       <c r="C1" s="5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>207</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -818,11 +835,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>